<commit_message>
User Role dodane i testy - cześć 1
</commit_message>
<xml_diff>
--- a/material/Konwencje.xlsx
+++ b/material/Konwencje.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojar\Documents\NAUKA\CODECOOL\DOGMATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojar\Documents\NAUKA\CODECOOL\GRANDE\DOGMAT-BACK\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA37AC95-45DD-4F76-B8D6-560F6BDC3CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBB650D-3D30-4488-B4AC-102AECCCB3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7C18D47-5F88-455C-8597-76E7D2D7D913}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C7C18D47-5F88-455C-8597-76E7D2D7D913}"/>
   </bookViews>
   <sheets>
     <sheet name="Anzliza 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Anzliza 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Założenia" sheetId="3" r:id="rId3"/>
-    <sheet name="Konwencja nazewnicza" sheetId="1" r:id="rId4"/>
+    <sheet name="Arkusz1" sheetId="5" r:id="rId2"/>
+    <sheet name="Anzliza 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Założenia" sheetId="3" r:id="rId4"/>
+    <sheet name="Konwencja nazewnicza" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Założenia!$A$2:$AL$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Założenia!$A$2:$AL$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="186">
   <si>
     <t>LP</t>
   </si>
@@ -531,12 +532,221 @@
   <si>
     <t>Realizcaja</t>
   </si>
+  <si>
+    <t>USER_ROLE</t>
+  </si>
+  <si>
+    <t>USER_TYPE</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>ENDPOINT</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>[ADMIN]</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>Lekarz</t>
+  </si>
+  <si>
+    <t>[DOCTOR]</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>Wojtek</t>
+  </si>
+  <si>
+    <t>[DOCTOR, SUPPLIER]</t>
+  </si>
+  <si>
+    <t>/about</t>
+  </si>
+  <si>
+    <t>Kasia</t>
+  </si>
+  <si>
+    <t>[TRAINER, SUPPLIER, USER]</t>
+  </si>
+  <si>
+    <t>/admin**</t>
+  </si>
+  <si>
+    <t>Piotr</t>
+  </si>
+  <si>
+    <t>[USER]</t>
+  </si>
+  <si>
+    <t>/training***</t>
+  </si>
+  <si>
+    <t>/doctor***</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>TRAINER</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>DOCTOR</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>PRINT</t>
+  </si>
+  <si>
+    <t>EXCEL</t>
+  </si>
+  <si>
+    <t>[READ, ADD, UPDATE, DELETE, PRINT,EXCEL]</t>
+  </si>
+  <si>
+    <t>[READ, ADD, UPDATE, PRINT]</t>
+  </si>
+  <si>
+    <t>[READ, ADD, UPDATE]</t>
+  </si>
+  <si>
+    <t>[READ]</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>[ADMIN, TRAINER]</t>
+  </si>
+  <si>
+    <t>[ADMIN, DOCTOR]</t>
+  </si>
+  <si>
+    <t>[ADMIN, USER]</t>
+  </si>
+  <si>
+    <t>/user***</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>REATE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>EAD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>PDATE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ELETE</t>
+    </r>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>USER_ROLE @ USER_TYPE</t>
+  </si>
+  <si>
+    <t>PONIŻEJ TABELA relacji ROLI i TYPU</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -602,8 +812,32 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +883,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,7 +1105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -996,6 +1242,25 @@
     <xf numFmtId="10" fontId="4" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1029,34 +1294,40 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="124">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1647,6 +1918,12 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -7232,7 +7509,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}" name="Tabela1" displayName="Tabela1" ref="A1:AA125" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}" name="Tabela1" displayName="Tabela1" ref="A1:AA125" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="A1:AA125" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA103">
     <sortCondition ref="C2:C103"/>
@@ -7249,7 +7526,7 @@
     <tableColumn id="21" xr3:uid="{14F95214-F7F7-4887-9E32-4AC8DF71F303}" name="Kryteria"/>
     <tableColumn id="7" xr3:uid="{008C15F0-14DC-4DCB-952A-08B7748666B8}" name="POLE BAZODANOWE"/>
     <tableColumn id="30" xr3:uid="{5DA97925-B338-4069-885C-930F3991709C}" name="Typ Pola"/>
-    <tableColumn id="22" xr3:uid="{B6C0EFE0-E131-4984-8B3F-A6319676F964}" name="Jest w Tabeli" dataDxfId="0"/>
+    <tableColumn id="22" xr3:uid="{B6C0EFE0-E131-4984-8B3F-A6319676F964}" name="Jest w Tabeli" dataDxfId="25"/>
     <tableColumn id="8" xr3:uid="{166ACF04-88DD-4931-AE2C-C5A643D4FD7A}" name="Kryteria dodatkowe"/>
     <tableColumn id="9" xr3:uid="{9EF33566-2E9B-4A03-AAC5-87669E20D085}" name="Klucz"/>
     <tableColumn id="10" xr3:uid="{E05A40AF-E589-48C0-9F21-08F2562FFB35}" name="RELACJA"/>
@@ -7573,7 +7850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB0B3C3-28BF-4F20-8534-1161614584E9}">
   <dimension ref="A3:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -7993,6 +8270,740 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAC5A2C-FFFA-47BF-A112-197EDBF0A44E}">
+  <dimension ref="A1:P38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2.5" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.83203125" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.83203125" customWidth="1"/>
+    <col min="15" max="15" width="20.5" customWidth="1"/>
+    <col min="16" max="16" width="1.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="72"/>
+      <c r="B1" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="78"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="72"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="72"/>
+      <c r="B2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="72"/>
+      <c r="E2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="72"/>
+      <c r="I2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" s="72"/>
+      <c r="M2" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="P2" s="72"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="72"/>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="72"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="72"/>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="72"/>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>149</v>
+      </c>
+      <c r="O3" t="s">
+        <v>174</v>
+      </c>
+      <c r="P3" s="72"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="72"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="72"/>
+      <c r="E4" s="4">
+        <f>E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="72"/>
+      <c r="I4" s="4">
+        <f>I3+1</f>
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L4" s="72"/>
+      <c r="M4" s="4">
+        <f>M3+1</f>
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" t="s">
+        <v>174</v>
+      </c>
+      <c r="P4" s="72"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="72"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="72"/>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E8" si="0">E4+1</f>
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5:I7" si="1">I4+1</f>
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="72"/>
+      <c r="M5" s="4">
+        <f t="shared" ref="M5:M9" si="2">M4+1</f>
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>155</v>
+      </c>
+      <c r="O5" t="s">
+        <v>174</v>
+      </c>
+      <c r="P5" s="72"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="72"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="72"/>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>156</v>
+      </c>
+      <c r="K6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="72"/>
+      <c r="M6" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>158</v>
+      </c>
+      <c r="O6" t="s">
+        <v>148</v>
+      </c>
+      <c r="P6" s="72"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="72"/>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="72"/>
+      <c r="I7" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" t="s">
+        <v>160</v>
+      </c>
+      <c r="L7" s="72"/>
+      <c r="M7" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>161</v>
+      </c>
+      <c r="O7" t="s">
+        <v>175</v>
+      </c>
+      <c r="P7" s="72"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="72"/>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="72"/>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>162</v>
+      </c>
+      <c r="O8" t="s">
+        <v>176</v>
+      </c>
+      <c r="P8" s="72"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="72"/>
+      <c r="B9" s="4">
+        <f>B8+1</f>
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="72"/>
+      <c r="E9" s="4"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="4">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>178</v>
+      </c>
+      <c r="O9" t="s">
+        <v>177</v>
+      </c>
+      <c r="P9" s="72"/>
+    </row>
+    <row r="10" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E11" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+    </row>
+    <row r="12" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="E13" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="E14" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="81"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E15" t="str">
+        <f>$F$3</f>
+        <v>ADMIN</v>
+      </c>
+      <c r="F15" t="str">
+        <f>$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G15" t="str">
+        <f>_xlfn.CONCAT("ROLE_",E15,"_",F15)</f>
+        <v>ROLE_ADMIN_CREATE</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f t="shared" ref="E16:E20" si="3">$F$3</f>
+        <v>ADMIN</v>
+      </c>
+      <c r="F16" t="str">
+        <f>$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16:G35" si="4">_xlfn.CONCAT("ROLE_",E16,"_",F16)</f>
+        <v>ROLE_ADMIN_READ</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>ADMIN</v>
+      </c>
+      <c r="F17" t="str">
+        <f>$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_ADMIN_UPDATE</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>ADMIN</v>
+      </c>
+      <c r="F18" t="str">
+        <f>$C$6</f>
+        <v>DELETE</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_ADMIN_DELETE</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>ADMIN</v>
+      </c>
+      <c r="F19" t="str">
+        <f>$C$7</f>
+        <v>PRINT</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_ADMIN_PRINT</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>ADMIN</v>
+      </c>
+      <c r="F20" t="str">
+        <f>$C$8</f>
+        <v>EXCEL</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_ADMIN_EXCEL</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E21" t="str">
+        <f>$F$4</f>
+        <v>TRAINER</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" ref="F21" si="5">$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_TRAINER_CREATE</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E22" t="str">
+        <f t="shared" ref="E22:E24" si="6">$F$4</f>
+        <v>TRAINER</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" ref="F22" si="7">$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_TRAINER_READ</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E23" t="str">
+        <f t="shared" si="6"/>
+        <v>TRAINER</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" ref="F23" si="8">$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_TRAINER_UPDATE</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E24" t="str">
+        <f t="shared" si="6"/>
+        <v>TRAINER</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" ref="F24" si="9">$C$7</f>
+        <v>PRINT</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_TRAINER_PRINT</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E25" t="str">
+        <f>$F$5</f>
+        <v>SUPPLIER</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" ref="F25" si="10">$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_SUPPLIER_CREATE</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E26" t="str">
+        <f t="shared" ref="E26:E28" si="11">$F$5</f>
+        <v>SUPPLIER</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" ref="F26" si="12">$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_SUPPLIER_READ</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E27" t="str">
+        <f t="shared" si="11"/>
+        <v>SUPPLIER</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" ref="F27" si="13">$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_SUPPLIER_UPDATE</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E28" t="str">
+        <f t="shared" si="11"/>
+        <v>SUPPLIER</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" ref="F28" si="14">$C$7</f>
+        <v>PRINT</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_SUPPLIER_PRINT</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E29" t="str">
+        <f>$F$6</f>
+        <v>DOCTOR</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" ref="F29" si="15">$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_DOCTOR_CREATE</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E30" t="str">
+        <f t="shared" ref="E30:E32" si="16">$F$6</f>
+        <v>DOCTOR</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" ref="F30" si="17">$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_DOCTOR_READ</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E31" t="str">
+        <f t="shared" si="16"/>
+        <v>DOCTOR</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" ref="F31" si="18">$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_DOCTOR_UPDATE</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E32" t="str">
+        <f t="shared" si="16"/>
+        <v>DOCTOR</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" ref="F32" si="19">$C$7</f>
+        <v>PRINT</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_DOCTOR_PRINT</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E33" t="str">
+        <f>$F$7</f>
+        <v>USER</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" ref="F33" si="20">$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_USER_CREATE</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E34" t="str">
+        <f t="shared" ref="E34:E35" si="21">$F$7</f>
+        <v>USER</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" ref="F34" si="22">$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_USER_READ</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E35" t="str">
+        <f t="shared" si="21"/>
+        <v>USER</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" ref="F35" si="23">$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="4"/>
+        <v>ROLE_USER_UPDATE</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E36" t="str">
+        <f>$F$8</f>
+        <v>GUEST</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" ref="F36" si="24">$C$3</f>
+        <v>CREATE</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" ref="G36:G38" si="25">_xlfn.CONCAT("ROLE_",E36,"_",F36)</f>
+        <v>ROLE_GUEST_CREATE</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E37" t="str">
+        <f t="shared" ref="E37:E38" si="26">$F$8</f>
+        <v>GUEST</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" ref="F37" si="27">$C$4</f>
+        <v>READ</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="25"/>
+        <v>ROLE_GUEST_READ</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E38" t="str">
+        <f t="shared" si="26"/>
+        <v>GUEST</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" ref="F38" si="28">$C$5</f>
+        <v>UPDATE</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="25"/>
+        <v>ROLE_GUEST_UPDATE</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98F56AF-0FBF-4148-86D6-676CB13F090E}">
   <dimension ref="A1:U19"/>
   <sheetViews>
@@ -8039,36 +9050,36 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="53" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="54" t="s">
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -9016,7 +10027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F251A146-35D4-4760-93E6-A9856726555B}">
   <dimension ref="A1:AM42"/>
   <sheetViews>
@@ -9044,46 +10055,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="57" t="s">
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="60" t="s">
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
-      <c r="AE1" s="61"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="61"/>
-      <c r="AH1" s="61"/>
-      <c r="AI1" s="61"/>
-      <c r="AJ1" s="61"/>
-      <c r="AK1" s="62"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="70"/>
+      <c r="AF1" s="70"/>
+      <c r="AG1" s="70"/>
+      <c r="AH1" s="70"/>
+      <c r="AI1" s="70"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="71"/>
     </row>
     <row r="2" spans="1:38" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -10652,13 +11663,13 @@
       <c r="AM24" s="41"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="52" t="s">
         <v>140</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="D25" s="56" t="s">
         <v>142</v>
       </c>
       <c r="E25" s="45" t="s">
@@ -10669,7 +11680,7 @@
       <c r="A26" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="64">
+      <c r="B26" s="53">
         <f>IF($C$31=0,0,C26/$C$31)</f>
         <v>0.66666666666666663</v>
       </c>
@@ -10677,7 +11688,7 @@
         <f>COUNTIF(C3:C23,A26)</f>
         <v>14</v>
       </c>
-      <c r="D26" s="68">
+      <c r="D26" s="57">
         <f>C26</f>
         <v>14</v>
       </c>
@@ -10690,7 +11701,7 @@
       <c r="A27" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="65">
+      <c r="B27" s="54">
         <f>IF($C$31=0,0,C27/$C$31)</f>
         <v>0</v>
       </c>
@@ -10698,7 +11709,7 @@
         <f>COUNTIF(C2:C22,A27)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="69">
+      <c r="D27" s="58">
         <f>C27</f>
         <v>0</v>
       </c>
@@ -10711,7 +11722,7 @@
       <c r="A28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="65">
+      <c r="B28" s="54">
         <f>IF($C$31=0,0,C28/$C$31)</f>
         <v>0</v>
       </c>
@@ -10719,7 +11730,7 @@
         <f>COUNTIF(C3:C23,A28)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="69">
+      <c r="D28" s="58">
         <f>C28</f>
         <v>0</v>
       </c>
@@ -10732,7 +11743,7 @@
       <c r="A29" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="65">
+      <c r="B29" s="54">
         <f t="shared" ref="B29:B30" si="3">IF($C$31=0,0,C29/$C$31)</f>
         <v>0.2857142857142857</v>
       </c>
@@ -10740,7 +11751,7 @@
         <f>COUNTIF(C4:C25,A29)</f>
         <v>6</v>
       </c>
-      <c r="D29" s="70"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -10750,7 +11761,7 @@
       <c r="A30" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="65">
+      <c r="B30" s="54">
         <f t="shared" si="3"/>
         <v>4.7619047619047616E-2</v>
       </c>
@@ -10758,7 +11769,7 @@
         <f>COUNTIF(C5:C26,A30)</f>
         <v>1</v>
       </c>
-      <c r="D30" s="70"/>
+      <c r="D30" s="59"/>
       <c r="E30" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -10768,7 +11779,7 @@
       <c r="A31" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="66">
+      <c r="B31" s="55">
         <f>SUM(B26:B28)</f>
         <v>0.66666666666666663</v>
       </c>
@@ -10906,105 +11917,105 @@
     <mergeCell ref="U1:AK1"/>
   </mergeCells>
   <conditionalFormatting sqref="A28:A31 C33:C34 B3:B24 B26 A27:B30">
-    <cfRule type="cellIs" dxfId="26" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="102" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="103" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J24">
-    <cfRule type="cellIs" dxfId="24" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="100" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="101" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="22" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="98" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="99" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="20" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="96" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="97" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:AK24 B26:B30 AJ24:AM24">
-    <cfRule type="cellIs" dxfId="18" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="37" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="38" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C24">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Arek"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Arek"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Arek"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E30">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E30">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11012,7 +12023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF88E9-A3E8-46CD-AC47-76C4FA16F352}">
   <dimension ref="A1:AA125"/>
   <sheetViews>

</xml_diff>

<commit_message>
Security zrobione dzięki MEGE pomocy mojego mantora Adama Arczyńskiegio - wielkie mu dzięki
</commit_message>
<xml_diff>
--- a/material/Konwencje.xlsx
+++ b/material/Konwencje.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojar\Documents\NAUKA\CODECOOL\GRANDE\DOGMAT-BACK\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBB650D-3D30-4488-B4AC-102AECCCB3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBEE840-30BE-4194-9A9A-AA5566BA9C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C7C18D47-5F88-455C-8597-76E7D2D7D913}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="190">
   <si>
     <t>LP</t>
   </si>
@@ -596,9 +596,6 @@
     <t>ADMIN</t>
   </si>
   <si>
-    <t>TRAINER</t>
-  </si>
-  <si>
     <t>SUPPLIER</t>
   </si>
   <si>
@@ -740,6 +737,21 @@
   </si>
   <si>
     <t>PONIŻEJ TABELA relacji ROLI i TYPU</t>
+  </si>
+  <si>
+    <t>CREATE</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
   </si>
 </sst>
 </file>
@@ -1261,6 +1273,34 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1294,40 +1334,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="116">
     <dxf>
       <fill>
         <patternFill>
@@ -1543,118 +1555,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -1818,106 +1718,14 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -6593,139 +6401,139 @@
     <pageField fld="2" hier="-1"/>
   </pageFields>
   <formats count="50">
-    <format dxfId="123">
+    <format dxfId="115">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="114">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="113">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="112">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="111">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="118">
+    <format dxfId="110">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="109">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="116">
+    <format dxfId="108">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="107">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="114">
+    <format dxfId="106">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="113">
+    <format dxfId="105">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="104">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="111">
+    <format dxfId="103">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="110">
+    <format dxfId="102">
       <pivotArea dataOnly="0" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="109">
+    <format dxfId="101">
       <pivotArea dataOnly="0" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="108">
+    <format dxfId="100">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="107">
+    <format dxfId="99">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="106">
+    <format dxfId="98">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="105">
+    <format dxfId="97">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="104">
+    <format dxfId="96">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="103">
+    <format dxfId="95">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="102">
+    <format dxfId="94">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="101">
+    <format dxfId="93">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="100">
+    <format dxfId="92">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="91">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="90">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="89">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="96">
+    <format dxfId="88">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="87">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="86">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="85">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="84">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="83">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="82">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="81">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="80">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="79">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="78">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="77">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="76">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="75">
       <pivotArea field="18" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="74">
       <pivotArea field="19" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="73">
       <pivotArea field="20" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="72">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="71">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1" selected="0" defaultSubtotal="1">
@@ -6734,7 +6542,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="70">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1" selected="0" defaultSubtotal="1">
@@ -6743,7 +6551,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="69">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1" selected="0" defaultSubtotal="1">
@@ -6752,7 +6560,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="68">
       <pivotArea outline="0" fieldPosition="0">
         <references count="5">
           <reference field="4" count="1" selected="0">
@@ -6773,7 +6581,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="67">
       <pivotArea outline="0" fieldPosition="0">
         <references count="5">
           <reference field="4" count="1" selected="0">
@@ -6794,7 +6602,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="66">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -7327,46 +7135,46 @@
     <dataField name="Liczba z POLE BAZODANOWE" fld="5" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="47">
-    <format dxfId="73">
+    <format dxfId="65">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="64">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="63">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="62">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="61">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="68">
+    <format dxfId="60">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="67">
+    <format dxfId="59">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="66">
+    <format dxfId="58">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="65">
+    <format dxfId="57">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="56">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="55">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="54">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="53">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="4">
@@ -7378,55 +7186,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="50">
       <pivotArea dataOnly="0" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="49">
       <pivotArea dataOnly="0" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="48">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="47">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="46">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="45">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="44">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="43">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="42">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="41">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="40">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="39">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="38">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="37">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="36">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="4">
@@ -7438,43 +7246,43 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="34">
       <pivotArea field="15" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="33">
       <pivotArea field="13" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="32">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="31">
       <pivotArea field="16" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="30">
       <pivotArea field="14" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="29">
       <pivotArea field="17" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="28">
       <pivotArea field="26" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="27">
       <pivotArea field="21" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="8"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="26">
       <pivotArea field="22" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="9"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="25">
       <pivotArea field="23" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="10"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="24">
       <pivotArea field="24" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="11"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="23">
       <pivotArea field="25" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="12"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="4">
@@ -7486,13 +7294,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="21">
       <pivotArea field="18" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="13"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="20">
       <pivotArea field="19" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="14"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="19">
       <pivotArea field="20" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="15"/>
     </format>
   </formats>
@@ -7509,7 +7317,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}" name="Tabela1" displayName="Tabela1" ref="A1:AA125" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}" name="Tabela1" displayName="Tabela1" ref="A1:AA125" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:AA125" xr:uid="{FA6C815C-5AA9-47DF-BFB5-75DB9BAE7CA7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA103">
     <sortCondition ref="C2:C103"/>
@@ -7526,7 +7334,7 @@
     <tableColumn id="21" xr3:uid="{14F95214-F7F7-4887-9E32-4AC8DF71F303}" name="Kryteria"/>
     <tableColumn id="7" xr3:uid="{008C15F0-14DC-4DCB-952A-08B7748666B8}" name="POLE BAZODANOWE"/>
     <tableColumn id="30" xr3:uid="{5DA97925-B338-4069-885C-930F3991709C}" name="Typ Pola"/>
-    <tableColumn id="22" xr3:uid="{B6C0EFE0-E131-4984-8B3F-A6319676F964}" name="Jest w Tabeli" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{B6C0EFE0-E131-4984-8B3F-A6319676F964}" name="Jest w Tabeli" dataDxfId="17"/>
     <tableColumn id="8" xr3:uid="{166ACF04-88DD-4931-AE2C-C5A643D4FD7A}" name="Kryteria dodatkowe"/>
     <tableColumn id="9" xr3:uid="{9EF33566-2E9B-4A03-AAC5-87669E20D085}" name="Klucz"/>
     <tableColumn id="10" xr3:uid="{E05A40AF-E589-48C0-9F21-08F2562FFB35}" name="RELACJA"/>
@@ -8274,7 +8082,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E33" sqref="E33:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8293,90 +8101,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="72"/>
-      <c r="B1" s="78" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="76" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="69" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="73" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="74" t="s">
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="72"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="61"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
+      <c r="A2" s="61"/>
       <c r="B2" s="60" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="72"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="60" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="72"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="60" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="L2" s="72"/>
+      <c r="L2" s="61"/>
       <c r="M2" s="60" t="s">
         <v>10</v>
       </c>
       <c r="N2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="77" t="s">
+      <c r="O2" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="P2" s="72"/>
+      <c r="P2" s="61"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="4">
-        <v>1</v>
+      <c r="A3" s="61"/>
+      <c r="B3">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="72"/>
+        <v>178</v>
+      </c>
+      <c r="D3" s="61"/>
       <c r="E3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>163</v>
       </c>
       <c r="G3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="72"/>
+        <v>169</v>
+      </c>
+      <c r="H3" s="61"/>
       <c r="I3" s="4">
         <v>1</v>
       </c>
@@ -8386,7 +8194,7 @@
       <c r="K3" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="72"/>
+      <c r="L3" s="61"/>
       <c r="M3" s="4">
         <v>1</v>
       </c>
@@ -8394,30 +8202,29 @@
         <v>149</v>
       </c>
       <c r="O3" t="s">
-        <v>174</v>
-      </c>
-      <c r="P3" s="72"/>
+        <v>173</v>
+      </c>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="4">
-        <v>2</v>
+      <c r="A4" s="61"/>
+      <c r="B4">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="72"/>
+        <v>179</v>
+      </c>
+      <c r="D4" s="61"/>
       <c r="E4" s="4">
-        <f>E3+1</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="G4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" s="72"/>
+        <v>170</v>
+      </c>
+      <c r="H4" s="61"/>
       <c r="I4" s="4">
         <f>I3+1</f>
         <v>2</v>
@@ -8428,7 +8235,7 @@
       <c r="K4" t="s">
         <v>151</v>
       </c>
-      <c r="L4" s="72"/>
+      <c r="L4" s="61"/>
       <c r="M4" s="4">
         <f>M3+1</f>
         <v>2</v>
@@ -8437,32 +8244,31 @@
         <v>152</v>
       </c>
       <c r="O4" t="s">
-        <v>174</v>
-      </c>
-      <c r="P4" s="72"/>
+        <v>173</v>
+      </c>
+      <c r="P4" s="61"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="4">
-        <v>3</v>
+      <c r="A5" s="61"/>
+      <c r="B5">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="72"/>
+        <v>180</v>
+      </c>
+      <c r="D5" s="61"/>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E8" si="0">E4+1</f>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" s="72"/>
+        <v>170</v>
+      </c>
+      <c r="H5" s="61"/>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I7" si="1">I4+1</f>
+        <f t="shared" ref="I5:I7" si="0">I4+1</f>
         <v>3</v>
       </c>
       <c r="J5" t="s">
@@ -8471,522 +8277,758 @@
       <c r="K5" t="s">
         <v>154</v>
       </c>
-      <c r="L5" s="72"/>
+      <c r="L5" s="61"/>
       <c r="M5" s="4">
-        <f t="shared" ref="M5:M9" si="2">M4+1</f>
+        <f t="shared" ref="M5:M9" si="1">M4+1</f>
         <v>3</v>
       </c>
       <c r="N5" t="s">
         <v>155</v>
       </c>
       <c r="O5" t="s">
-        <v>174</v>
-      </c>
-      <c r="P5" s="72"/>
+        <v>173</v>
+      </c>
+      <c r="P5" s="61"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="4">
-        <v>4</v>
+      <c r="A6" s="61"/>
+      <c r="B6">
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D6" s="72"/>
+        <v>181</v>
+      </c>
+      <c r="D6" s="61"/>
       <c r="E6" s="4">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="61"/>
+      <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="4">
+      <c r="J6" t="s">
+        <v>156</v>
+      </c>
+      <c r="K6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="61"/>
+      <c r="M6" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K6" t="s">
-        <v>157</v>
-      </c>
-      <c r="L6" s="72"/>
-      <c r="M6" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
       <c r="N6" t="s">
         <v>158</v>
       </c>
       <c r="O6" t="s">
         <v>148</v>
       </c>
-      <c r="P6" s="72"/>
+      <c r="P6" s="61"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="72"/>
-      <c r="B7" s="4">
-        <v>5</v>
+      <c r="A7" s="61"/>
+      <c r="B7">
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="72"/>
+        <v>167</v>
+      </c>
+      <c r="D7" s="61"/>
       <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" s="61"/>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="4">
+      <c r="J7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" t="s">
+        <v>160</v>
+      </c>
+      <c r="L7" s="61"/>
+      <c r="M7" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J7" t="s">
-        <v>159</v>
-      </c>
-      <c r="K7" t="s">
-        <v>160</v>
-      </c>
-      <c r="L7" s="72"/>
-      <c r="M7" s="4">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
       <c r="N7" t="s">
         <v>161</v>
       </c>
       <c r="O7" t="s">
-        <v>175</v>
-      </c>
-      <c r="P7" s="72"/>
+        <v>174</v>
+      </c>
+      <c r="P7" s="61"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="72"/>
-      <c r="B8" s="4">
-        <v>6</v>
+      <c r="A8" s="61"/>
+      <c r="B8">
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="72"/>
+        <v>168</v>
+      </c>
+      <c r="D8" s="61"/>
       <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="L8" s="72"/>
+      <c r="L8" s="61"/>
       <c r="M8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N8" t="s">
         <v>162</v>
       </c>
       <c r="O8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P8" s="61"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="4"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>177</v>
+      </c>
+      <c r="O9" t="s">
         <v>176</v>
       </c>
-      <c r="P8" s="72"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="72"/>
-      <c r="B9" s="4">
-        <f>B8+1</f>
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="4"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="4">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="N9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O9" t="s">
-        <v>177</v>
-      </c>
-      <c r="P9" s="72"/>
+      <c r="P9" s="61"/>
     </row>
     <row r="10" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E11" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
+      <c r="E11" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
     </row>
     <row r="12" spans="1:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E13" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
+      <c r="E13" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="I13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="G14" s="81"/>
+      <c r="G14" s="64"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E15" t="str">
-        <f>$F$3</f>
+      <c r="B15" t="str">
+        <f t="shared" ref="B15:B20" si="2">$F$3</f>
         <v>ADMIN</v>
       </c>
-      <c r="F15" t="str">
+      <c r="C15" t="str">
         <f>$C$3</f>
         <v>CREATE</v>
       </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E20" si="3">$E$3</f>
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <f>$B$3</f>
+        <v>8</v>
+      </c>
       <c r="G15" t="str">
-        <f>_xlfn.CONCAT("ROLE_",E15,"_",F15)</f>
-        <v>ROLE_ADMIN_CREATE</v>
+        <f>_xlfn.CONCAT(B15,"_",C15)</f>
+        <v>ADMIN_CREATE</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E16" t="str">
-        <f t="shared" ref="E16:E20" si="3">$F$3</f>
+      <c r="B16" t="str">
+        <f t="shared" si="2"/>
         <v>ADMIN</v>
       </c>
-      <c r="F16" t="str">
+      <c r="C16" t="str">
         <f>$C$4</f>
         <v>READ</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <f>$B$4</f>
+        <v>9</v>
+      </c>
       <c r="G16" t="str">
-        <f t="shared" ref="G16:G35" si="4">_xlfn.CONCAT("ROLE_",E16,"_",F16)</f>
-        <v>ROLE_ADMIN_READ</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G16:G38" si="4">_xlfn.CONCAT(B16,"_",C16)</f>
+        <v>ADMIN_READ</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" t="str">
+        <f t="shared" si="2"/>
         <v>ADMIN</v>
       </c>
-      <c r="F17" t="str">
+      <c r="C17" t="str">
         <f>$C$5</f>
         <v>UPDATE</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f>$B$5</f>
+        <v>15</v>
+      </c>
       <c r="G17" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_ADMIN_UPDATE</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E18" t="str">
-        <f t="shared" si="3"/>
+        <v>ADMIN_UPDATE</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" t="str">
+        <f t="shared" si="2"/>
         <v>ADMIN</v>
       </c>
-      <c r="F18" t="str">
+      <c r="C18" t="str">
         <f>$C$6</f>
         <v>DELETE</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f>$B$6</f>
+        <v>11</v>
+      </c>
       <c r="G18" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_ADMIN_DELETE</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E19" t="str">
-        <f t="shared" si="3"/>
+        <v>ADMIN_DELETE</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" t="str">
+        <f t="shared" si="2"/>
         <v>ADMIN</v>
       </c>
-      <c r="F19" t="str">
+      <c r="C19" t="str">
         <f>$C$7</f>
         <v>PRINT</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f>$B$7</f>
+        <v>12</v>
+      </c>
       <c r="G19" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_ADMIN_PRINT</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E20" t="str">
-        <f t="shared" si="3"/>
+        <v>ADMIN_PRINT</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" t="str">
+        <f t="shared" si="2"/>
         <v>ADMIN</v>
       </c>
-      <c r="F20" t="str">
+      <c r="C20" t="str">
         <f>$C$8</f>
         <v>EXCEL</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f>$B$8</f>
+        <v>13</v>
+      </c>
       <c r="G20" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_ADMIN_EXCEL</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E21" t="str">
+        <v>ADMIN_EXCEL</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" t="str">
         <f>$F$4</f>
-        <v>TRAINER</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" ref="F21" si="5">$C$3</f>
+        <v>MANAGER</v>
+      </c>
+      <c r="C21" t="str">
+        <f>$C$3</f>
         <v>CREATE</v>
+      </c>
+      <c r="E21">
+        <f>$E$4</f>
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <f>$B$3</f>
+        <v>8</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_TRAINER_CREATE</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E22" t="str">
-        <f t="shared" ref="E22:E24" si="6">$F$4</f>
-        <v>TRAINER</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" ref="F22" si="7">$C$4</f>
+        <v>MANAGER_CREATE</v>
+      </c>
+      <c r="J21">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" t="str">
+        <f>$F$4</f>
+        <v>MANAGER</v>
+      </c>
+      <c r="C22" t="str">
+        <f>$C$4</f>
         <v>READ</v>
+      </c>
+      <c r="E22">
+        <f>$E$4</f>
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <f>$B$4</f>
+        <v>9</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_TRAINER_READ</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E23" t="str">
-        <f t="shared" si="6"/>
-        <v>TRAINER</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" ref="F23" si="8">$C$5</f>
+        <v>MANAGER_READ</v>
+      </c>
+      <c r="J22">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" t="str">
+        <f>$F$4</f>
+        <v>MANAGER</v>
+      </c>
+      <c r="C23" t="str">
+        <f>$C$5</f>
         <v>UPDATE</v>
+      </c>
+      <c r="E23">
+        <f>$E$4</f>
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <f>$B$5</f>
+        <v>15</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_TRAINER_UPDATE</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E24" t="str">
-        <f t="shared" si="6"/>
-        <v>TRAINER</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" ref="F24" si="9">$C$7</f>
+        <v>MANAGER_UPDATE</v>
+      </c>
+      <c r="J23">
+        <v>12</v>
+      </c>
+      <c r="K23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" t="str">
+        <f>$F$4</f>
+        <v>MANAGER</v>
+      </c>
+      <c r="C24" t="str">
+        <f>$C$7</f>
         <v>PRINT</v>
+      </c>
+      <c r="E24">
+        <f>$E$4</f>
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <f>$B$7</f>
+        <v>12</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_TRAINER_PRINT</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E25" t="str">
+        <v>MANAGER_PRINT</v>
+      </c>
+      <c r="J24">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" t="str">
         <f>$F$5</f>
         <v>SUPPLIER</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" ref="F25" si="10">$C$3</f>
+      <c r="C25" t="str">
+        <f>$C$3</f>
         <v>CREATE</v>
+      </c>
+      <c r="E25">
+        <f>$E$5</f>
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <f>$B$3</f>
+        <v>8</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_SUPPLIER_CREATE</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E26" t="str">
-        <f t="shared" ref="E26:E28" si="11">$F$5</f>
+        <v>SUPPLIER_CREATE</v>
+      </c>
+      <c r="J25">
+        <v>14</v>
+      </c>
+      <c r="K25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" t="str">
+        <f>$F$5</f>
         <v>SUPPLIER</v>
       </c>
-      <c r="F26" t="str">
-        <f t="shared" ref="F26" si="12">$C$4</f>
+      <c r="C26" t="str">
+        <f>$C$4</f>
         <v>READ</v>
+      </c>
+      <c r="E26">
+        <f>$E$5</f>
+        <v>17</v>
+      </c>
+      <c r="F26">
+        <f>$B$4</f>
+        <v>9</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_SUPPLIER_READ</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E27" t="str">
-        <f t="shared" si="11"/>
+        <v>SUPPLIER_READ</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" t="str">
+        <f>$F$5</f>
         <v>SUPPLIER</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" ref="F27" si="13">$C$5</f>
+      <c r="C27" t="str">
+        <f>$C$5</f>
         <v>UPDATE</v>
+      </c>
+      <c r="E27">
+        <f>$E$5</f>
+        <v>17</v>
+      </c>
+      <c r="F27">
+        <f>$B$5</f>
+        <v>15</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_SUPPLIER_UPDATE</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E28" t="str">
-        <f t="shared" si="11"/>
+        <v>SUPPLIER_UPDATE</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="str">
+        <f>$F$5</f>
         <v>SUPPLIER</v>
       </c>
-      <c r="F28" t="str">
-        <f t="shared" ref="F28" si="14">$C$7</f>
+      <c r="C28" t="str">
+        <f>$C$7</f>
         <v>PRINT</v>
+      </c>
+      <c r="E28">
+        <f>$E$5</f>
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <f>$B$7</f>
+        <v>12</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_SUPPLIER_PRINT</v>
-      </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E29" t="str">
+        <v>SUPPLIER_PRINT</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" t="str">
         <f>$F$6</f>
         <v>DOCTOR</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" ref="F29" si="15">$C$3</f>
+      <c r="C29" t="str">
+        <f>$C$3</f>
         <v>CREATE</v>
+      </c>
+      <c r="E29">
+        <f>$E$6</f>
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <f>$B$3</f>
+        <v>8</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_DOCTOR_CREATE</v>
-      </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E30" t="str">
-        <f t="shared" ref="E30:E32" si="16">$F$6</f>
+        <v>DOCTOR_CREATE</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" t="str">
+        <f>$F$6</f>
         <v>DOCTOR</v>
       </c>
-      <c r="F30" t="str">
-        <f t="shared" ref="F30" si="17">$C$4</f>
+      <c r="C30" t="str">
+        <f>$C$4</f>
         <v>READ</v>
+      </c>
+      <c r="E30">
+        <f>$E$6</f>
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <f>$B$4</f>
+        <v>9</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_DOCTOR_READ</v>
-      </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E31" t="str">
-        <f t="shared" si="16"/>
+        <v>DOCTOR_READ</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" t="str">
+        <f>$F$6</f>
         <v>DOCTOR</v>
       </c>
-      <c r="F31" t="str">
-        <f t="shared" ref="F31" si="18">$C$5</f>
+      <c r="C31" t="str">
+        <f>$C$5</f>
         <v>UPDATE</v>
+      </c>
+      <c r="E31">
+        <f>$E$6</f>
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <f>$B$5</f>
+        <v>15</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_DOCTOR_UPDATE</v>
-      </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E32" t="str">
-        <f t="shared" si="16"/>
+        <v>DOCTOR_UPDATE</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" t="str">
+        <f>$F$6</f>
         <v>DOCTOR</v>
       </c>
-      <c r="F32" t="str">
-        <f t="shared" ref="F32" si="19">$C$7</f>
+      <c r="C32" t="str">
+        <f>$C$7</f>
         <v>PRINT</v>
+      </c>
+      <c r="E32">
+        <f>$E$6</f>
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <f>$B$7</f>
+        <v>12</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_DOCTOR_PRINT</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E33" t="str">
+        <v>DOCTOR_PRINT</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" t="str">
         <f>$F$7</f>
         <v>USER</v>
       </c>
-      <c r="F33" t="str">
-        <f t="shared" ref="F33" si="20">$C$3</f>
+      <c r="C33" t="str">
+        <f>$C$3</f>
         <v>CREATE</v>
+      </c>
+      <c r="E33">
+        <f>$E$7</f>
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f>$B$3</f>
+        <v>8</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_USER_CREATE</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E34" t="str">
-        <f t="shared" ref="E34:E35" si="21">$F$7</f>
+        <v>USER_CREATE</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" t="str">
+        <f>$F$7</f>
         <v>USER</v>
       </c>
-      <c r="F34" t="str">
-        <f t="shared" ref="F34" si="22">$C$4</f>
+      <c r="C34" t="str">
+        <f>$C$4</f>
         <v>READ</v>
+      </c>
+      <c r="E34">
+        <f>$E$7</f>
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f>$B$4</f>
+        <v>9</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_USER_READ</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E35" t="str">
-        <f t="shared" si="21"/>
+        <v>USER_READ</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" t="str">
+        <f>$F$7</f>
         <v>USER</v>
       </c>
-      <c r="F35" t="str">
-        <f t="shared" ref="F35" si="23">$C$5</f>
+      <c r="C35" t="str">
+        <f>$C$5</f>
         <v>UPDATE</v>
+      </c>
+      <c r="E35">
+        <f>$E$7</f>
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <f>$B$5</f>
+        <v>15</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="4"/>
-        <v>ROLE_USER_UPDATE</v>
-      </c>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E36" t="str">
+        <v>USER_UPDATE</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" t="str">
         <f>$F$8</f>
         <v>GUEST</v>
       </c>
-      <c r="F36" t="str">
-        <f t="shared" ref="F36" si="24">$C$3</f>
+      <c r="C36" t="str">
+        <f>$C$3</f>
         <v>CREATE</v>
       </c>
+      <c r="E36">
+        <f>$E$8</f>
+        <v>19</v>
+      </c>
+      <c r="F36">
+        <f>$B$3</f>
+        <v>8</v>
+      </c>
       <c r="G36" t="str">
-        <f t="shared" ref="G36:G38" si="25">_xlfn.CONCAT("ROLE_",E36,"_",F36)</f>
-        <v>ROLE_GUEST_CREATE</v>
-      </c>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E37" t="str">
-        <f t="shared" ref="E37:E38" si="26">$F$8</f>
+        <f t="shared" si="4"/>
+        <v>GUEST_CREATE</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" t="str">
+        <f>$F$8</f>
         <v>GUEST</v>
       </c>
-      <c r="F37" t="str">
-        <f t="shared" ref="F37" si="27">$C$4</f>
+      <c r="C37" t="str">
+        <f>$C$4</f>
         <v>READ</v>
       </c>
+      <c r="E37">
+        <f>$E$8</f>
+        <v>19</v>
+      </c>
+      <c r="F37">
+        <f>$B$4</f>
+        <v>9</v>
+      </c>
       <c r="G37" t="str">
-        <f t="shared" si="25"/>
-        <v>ROLE_GUEST_READ</v>
-      </c>
-    </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E38" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="4"/>
+        <v>GUEST_READ</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" t="str">
+        <f>$F$8</f>
         <v>GUEST</v>
       </c>
-      <c r="F38" t="str">
-        <f t="shared" ref="F38" si="28">$C$5</f>
+      <c r="C38" t="str">
+        <f>$C$5</f>
         <v>UPDATE</v>
       </c>
+      <c r="E38">
+        <f>$E$8</f>
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <f>$B$5</f>
+        <v>15</v>
+      </c>
       <c r="G38" t="str">
-        <f t="shared" si="25"/>
-        <v>ROLE_GUEST_UPDATE</v>
+        <f t="shared" si="4"/>
+        <v>GUEST_UPDATE</v>
       </c>
     </row>
   </sheetData>
@@ -9050,36 +9092,36 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
       <c r="H3" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62" t="s">
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="63" t="s">
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -10055,46 +10097,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66" t="s">
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="69" t="s">
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="71"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="81"/>
     </row>
     <row r="2" spans="1:38" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -11916,102 +11958,66 @@
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="U1:AK1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A28:A31 C33:C34 B3:B24 B26 A27:B30">
-    <cfRule type="cellIs" dxfId="24" priority="102" operator="equal">
+  <conditionalFormatting sqref="A26">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>"Arek"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J24">
-    <cfRule type="cellIs" dxfId="22" priority="100" operator="equal">
+  <conditionalFormatting sqref="A27:B30 A28:A31 C33:C34">
+    <cfRule type="cellIs" dxfId="13" priority="102" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="103" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="20" priority="98" operator="equal">
+  <conditionalFormatting sqref="B3:AK24 AJ24:AM24 B26:B30">
+    <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="99" operator="equal">
-      <formula>"Tak"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="18" priority="96" operator="equal">
-      <formula>"Nie"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="97" operator="equal">
-      <formula>"Tak"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:AK24 B26:B30 AJ24:AM24">
-    <cfRule type="cellIs" dxfId="16" priority="37" operator="equal">
-      <formula>"Nie"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="38" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C24">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"Arek"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
-      <formula>"Nie"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
-      <formula>"Tak"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
-      <formula>"Arek"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"Nie"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Arek"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="D25">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="D36:E36">
+    <cfRule type="cellIs" dxfId="3" priority="96" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="97" operator="equal">
       <formula>"Tak"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E30">
+  <conditionalFormatting sqref="E25:E30">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Nie"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Kolejna partia po rewizji na froncie
</commit_message>
<xml_diff>
--- a/material/Konwencje.xlsx
+++ b/material/Konwencje.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojar\Documents\NAUKA\CODECOOL\GRANDE\DOGMAT-BACK\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBEE840-30BE-4194-9A9A-AA5566BA9C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C18C9DA-35D8-4946-B09A-8B11B4ABC800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C7C18D47-5F88-455C-8597-76E7D2D7D913}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C7C18D47-5F88-455C-8597-76E7D2D7D913}"/>
   </bookViews>
   <sheets>
     <sheet name="Anzliza 1" sheetId="4" r:id="rId1"/>
     <sheet name="Arkusz1" sheetId="5" r:id="rId2"/>
-    <sheet name="Anzliza 2" sheetId="2" r:id="rId3"/>
-    <sheet name="Założenia" sheetId="3" r:id="rId4"/>
-    <sheet name="Konwencja nazewnicza" sheetId="1" r:id="rId5"/>
+    <sheet name="UPRAWNIENIA" sheetId="6" r:id="rId3"/>
+    <sheet name="Anzliza 2" sheetId="2" r:id="rId4"/>
+    <sheet name="Założenia" sheetId="3" r:id="rId5"/>
+    <sheet name="Konwencja nazewnicza" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Założenia!$A$2:$AL$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Założenia!$A$2:$AL$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="212">
   <si>
     <t>LP</t>
   </si>
@@ -753,6 +754,72 @@
   <si>
     <t>MANAGER</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TRENER</t>
+  </si>
+  <si>
+    <t>ANIAMLTYPES</t>
+  </si>
+  <si>
+    <t>ANIAML</t>
+  </si>
+  <si>
+    <t>BREED</t>
+  </si>
+  <si>
+    <t>TRAINING</t>
+  </si>
+  <si>
+    <t>TRAININGSTEPS</t>
+  </si>
+  <si>
+    <t>USERANIMAL</t>
+  </si>
+  <si>
+    <t>CAREANNOUNCEMENT</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TIMEUNITS</t>
+  </si>
+  <si>
+    <t>VOIVODESHIP</t>
+  </si>
+  <si>
+    <t>PROVINCES</t>
+  </si>
+  <si>
+    <t>CITIES</t>
+  </si>
+  <si>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>PROVILAGES</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>UU</t>
+  </si>
+  <si>
+    <t>NAZWA</t>
+  </si>
+  <si>
+    <t>KATEGORIA</t>
+  </si>
+  <si>
+    <t>DOBAZY</t>
+  </si>
 </sst>
 </file>
 
@@ -1117,7 +1184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1332,6 +1399,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8081,7 +8151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAC5A2C-FFFA-47BF-A112-197EDBF0A44E}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33:F35"/>
     </sheetView>
   </sheetViews>
@@ -9046,6 +9116,2715 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4617B5A5-21B6-427F-AE39-378BFB59ACB7}">
+  <dimension ref="A1:K92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="82" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="82" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="82" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="82" t="s">
+        <v>208</v>
+      </c>
+      <c r="K1" s="82" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(A2,"-",B2)</f>
+        <v>ANIAMLTYPES-CREATE</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(A3,"-",B3)</f>
+        <v>ANIAMLTYPES-READ</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f>D3</f>
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(A4,"-",B4)</f>
+        <v>ANIAMLTYPES-UPDATE</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(A5,"-",B5)</f>
+        <v>ANIAMLTYPES-DELETE</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(A6,"-",B6)</f>
+        <v>ANIAMLTYPES-EXCEL</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(A7,"-",B7)</f>
+        <v>ANIAMLTYPES-PRINT</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(A8,"-",B8)</f>
+        <v>ANIAMLTYPES-PDF</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(A9,"-",B9)</f>
+        <v>ANIAML-CREATE</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(A10,"-",B10)</f>
+        <v>ANIAML-READ</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f>D10</f>
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(A11,"-",B11)</f>
+        <v>ANIAML-UPDATE</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11">
+        <v>19</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(A12,"-",B12)</f>
+        <v>ANIAML-DELETE</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>199</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(A13,"-",B13)</f>
+        <v>ANIAML-EXCEL</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>199</v>
+      </c>
+      <c r="H13">
+        <v>21</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(A14,"-",B14)</f>
+        <v>ANIAML-PRINT</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(A15,"-",B15)</f>
+        <v>ANIAML-PDF</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H15">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="K15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(A16,"-",B16)</f>
+        <v>BREED-CREATE</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>199</v>
+      </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xlfn.CONCAT(A17,"-",B17)</f>
+        <v>BREED-READ</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>21</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f>D17</f>
+        <v>21</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT(A18,"-",B18)</f>
+        <v>BREED-UPDATE</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H18">
+        <v>25</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(A19,"-",B19)</f>
+        <v>BREED-DELETE</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>199</v>
+      </c>
+      <c r="H19">
+        <v>26</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(A20,"-",B20)</f>
+        <v>BREED-EXCEL</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20">
+        <v>63</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(A21,"-",B21)</f>
+        <v>BREED-PRINT</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21">
+        <v>70</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" t="str">
+        <f>_xlfn.CONCAT(A22,"-",B22)</f>
+        <v>BREED-PDF</v>
+      </c>
+      <c r="D22">
+        <v>26</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22">
+        <v>77</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>204</v>
+      </c>
+      <c r="B23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(A23,"-",B23)</f>
+        <v>ROLE-CREATE</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>199</v>
+      </c>
+      <c r="I23" t="s">
+        <v>199</v>
+      </c>
+      <c r="K23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT(A24,"-",B24)</f>
+        <v>ROLE-READ</v>
+      </c>
+      <c r="D24">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>199</v>
+      </c>
+      <c r="I24" t="s">
+        <v>199</v>
+      </c>
+      <c r="K24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT(A25,"-",B25)</f>
+        <v>ROLE-UPDATE</v>
+      </c>
+      <c r="D25">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>199</v>
+      </c>
+      <c r="I25" t="s">
+        <v>199</v>
+      </c>
+      <c r="K25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" t="str">
+        <f>_xlfn.CONCAT(A26,"-",B26)</f>
+        <v>ROLE-DELETE</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I26" t="s">
+        <v>199</v>
+      </c>
+      <c r="K26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" t="str">
+        <f>_xlfn.CONCAT(A27,"-",B27)</f>
+        <v>ROLE-EXCEL</v>
+      </c>
+      <c r="D27">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>199</v>
+      </c>
+      <c r="I27" t="s">
+        <v>199</v>
+      </c>
+      <c r="K27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="str">
+        <f>_xlfn.CONCAT(A28,"-",B28)</f>
+        <v>ROLE-PRINT</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>199</v>
+      </c>
+      <c r="I28" t="s">
+        <v>199</v>
+      </c>
+      <c r="K28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" t="str">
+        <f>_xlfn.CONCAT(A29,"-",B29)</f>
+        <v>ROLE-PDF</v>
+      </c>
+      <c r="D29">
+        <v>33</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>199</v>
+      </c>
+      <c r="I29" t="s">
+        <v>199</v>
+      </c>
+      <c r="K29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" t="s">
+        <v>185</v>
+      </c>
+      <c r="C30" t="str">
+        <f>_xlfn.CONCAT(A30,"-",B30)</f>
+        <v>PROVILAGES-CREATE</v>
+      </c>
+      <c r="D30">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>199</v>
+      </c>
+      <c r="I30" t="s">
+        <v>199</v>
+      </c>
+      <c r="K30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" t="str">
+        <f>_xlfn.CONCAT(A31,"-",B31)</f>
+        <v>PROVILAGES-READ</v>
+      </c>
+      <c r="D31">
+        <v>35</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>199</v>
+      </c>
+      <c r="I31" t="s">
+        <v>199</v>
+      </c>
+      <c r="K31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" t="str">
+        <f>_xlfn.CONCAT(A32,"-",B32)</f>
+        <v>PROVILAGES-UPDATE</v>
+      </c>
+      <c r="D32">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>199</v>
+      </c>
+      <c r="I32" t="s">
+        <v>199</v>
+      </c>
+      <c r="K32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" t="str">
+        <f>_xlfn.CONCAT(A33,"-",B33)</f>
+        <v>PROVILAGES-DELETE</v>
+      </c>
+      <c r="D33">
+        <v>37</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>199</v>
+      </c>
+      <c r="I33" t="s">
+        <v>199</v>
+      </c>
+      <c r="K33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" t="str">
+        <f>_xlfn.CONCAT(A34,"-",B34)</f>
+        <v>PROVILAGES-EXCEL</v>
+      </c>
+      <c r="D34">
+        <v>38</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>199</v>
+      </c>
+      <c r="I34" t="s">
+        <v>199</v>
+      </c>
+      <c r="K34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="str">
+        <f>_xlfn.CONCAT(A35,"-",B35)</f>
+        <v>PROVILAGES-PRINT</v>
+      </c>
+      <c r="D35">
+        <v>39</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>199</v>
+      </c>
+      <c r="I35" t="s">
+        <v>199</v>
+      </c>
+      <c r="K35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" t="str">
+        <f>_xlfn.CONCAT(A36,"-",B36)</f>
+        <v>PROVILAGES-PDF</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>199</v>
+      </c>
+      <c r="I36" t="s">
+        <v>199</v>
+      </c>
+      <c r="K36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C37" t="str">
+        <f>_xlfn.CONCAT(A37,"-",B37)</f>
+        <v>VOIVODESHIP-CREATE</v>
+      </c>
+      <c r="D37">
+        <v>41</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>199</v>
+      </c>
+      <c r="I37" t="s">
+        <v>199</v>
+      </c>
+      <c r="K37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" t="str">
+        <f>_xlfn.CONCAT(A38,"-",B38)</f>
+        <v>VOIVODESHIP-READ</v>
+      </c>
+      <c r="D38">
+        <v>42</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>199</v>
+      </c>
+      <c r="I38" t="s">
+        <v>199</v>
+      </c>
+      <c r="J38">
+        <f>D38</f>
+        <v>42</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" t="str">
+        <f>_xlfn.CONCAT(A39,"-",B39)</f>
+        <v>VOIVODESHIP-UPDATE</v>
+      </c>
+      <c r="D39">
+        <v>43</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>199</v>
+      </c>
+      <c r="I39" t="s">
+        <v>199</v>
+      </c>
+      <c r="K39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" t="str">
+        <f>_xlfn.CONCAT(A40,"-",B40)</f>
+        <v>VOIVODESHIP-DELETE</v>
+      </c>
+      <c r="D40">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>199</v>
+      </c>
+      <c r="I40" t="s">
+        <v>199</v>
+      </c>
+      <c r="K40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" t="str">
+        <f>_xlfn.CONCAT(A41,"-",B41)</f>
+        <v>VOIVODESHIP-EXCEL</v>
+      </c>
+      <c r="D41">
+        <v>45</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>199</v>
+      </c>
+      <c r="I41" t="s">
+        <v>199</v>
+      </c>
+      <c r="K41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" t="str">
+        <f>_xlfn.CONCAT(A42,"-",B42)</f>
+        <v>VOIVODESHIP-PRINT</v>
+      </c>
+      <c r="D42">
+        <v>46</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>199</v>
+      </c>
+      <c r="I42" t="s">
+        <v>199</v>
+      </c>
+      <c r="K42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" t="str">
+        <f>_xlfn.CONCAT(A43,"-",B43)</f>
+        <v>VOIVODESHIP-PDF</v>
+      </c>
+      <c r="D43">
+        <v>47</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="s">
+        <v>199</v>
+      </c>
+      <c r="I43" t="s">
+        <v>199</v>
+      </c>
+      <c r="K43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" t="str">
+        <f>_xlfn.CONCAT(A44,"-",B44)</f>
+        <v>PROVINCES-CREATE</v>
+      </c>
+      <c r="D44">
+        <v>48</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>199</v>
+      </c>
+      <c r="I44" t="s">
+        <v>199</v>
+      </c>
+      <c r="K44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" t="str">
+        <f>_xlfn.CONCAT(A45,"-",B45)</f>
+        <v>PROVINCES-READ</v>
+      </c>
+      <c r="D45">
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="G45" t="s">
+        <v>199</v>
+      </c>
+      <c r="I45" t="s">
+        <v>199</v>
+      </c>
+      <c r="J45">
+        <f>D45</f>
+        <v>49</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" t="str">
+        <f>_xlfn.CONCAT(A46,"-",B46)</f>
+        <v>PROVINCES-UPDATE</v>
+      </c>
+      <c r="D46">
+        <v>50</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>199</v>
+      </c>
+      <c r="I46" t="s">
+        <v>199</v>
+      </c>
+      <c r="K46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" t="str">
+        <f>_xlfn.CONCAT(A47,"-",B47)</f>
+        <v>PROVINCES-DELETE</v>
+      </c>
+      <c r="D47">
+        <v>51</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>199</v>
+      </c>
+      <c r="I47" t="s">
+        <v>199</v>
+      </c>
+      <c r="K47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" t="str">
+        <f>_xlfn.CONCAT(A48,"-",B48)</f>
+        <v>PROVINCES-EXCEL</v>
+      </c>
+      <c r="D48">
+        <v>52</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="s">
+        <v>199</v>
+      </c>
+      <c r="I48" t="s">
+        <v>199</v>
+      </c>
+      <c r="K48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" t="str">
+        <f>_xlfn.CONCAT(A49,"-",B49)</f>
+        <v>PROVINCES-PRINT</v>
+      </c>
+      <c r="D49">
+        <v>53</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>199</v>
+      </c>
+      <c r="I49" t="s">
+        <v>199</v>
+      </c>
+      <c r="K49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>202</v>
+      </c>
+      <c r="B50" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" t="str">
+        <f>_xlfn.CONCAT(A50,"-",B50)</f>
+        <v>PROVINCES-PDF</v>
+      </c>
+      <c r="D50">
+        <v>54</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>199</v>
+      </c>
+      <c r="I50" t="s">
+        <v>199</v>
+      </c>
+      <c r="K50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" t="str">
+        <f>_xlfn.CONCAT(A51,"-",B51)</f>
+        <v>CITIES-CREATE</v>
+      </c>
+      <c r="D51">
+        <v>55</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>199</v>
+      </c>
+      <c r="I51" t="s">
+        <v>199</v>
+      </c>
+      <c r="K51" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>203</v>
+      </c>
+      <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="str">
+        <f>_xlfn.CONCAT(A52,"-",B52)</f>
+        <v>CITIES-READ</v>
+      </c>
+      <c r="D52">
+        <v>56</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>199</v>
+      </c>
+      <c r="I52" t="s">
+        <v>199</v>
+      </c>
+      <c r="J52">
+        <f>D52</f>
+        <v>56</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53" t="str">
+        <f>_xlfn.CONCAT(A53,"-",B53)</f>
+        <v>CITIES-UPDATE</v>
+      </c>
+      <c r="D53">
+        <v>57</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>199</v>
+      </c>
+      <c r="I53" t="s">
+        <v>199</v>
+      </c>
+      <c r="K53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="str">
+        <f>_xlfn.CONCAT(A54,"-",B54)</f>
+        <v>CITIES-DELETE</v>
+      </c>
+      <c r="D54">
+        <v>58</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>199</v>
+      </c>
+      <c r="I54" t="s">
+        <v>199</v>
+      </c>
+      <c r="K54" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>203</v>
+      </c>
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" t="str">
+        <f>_xlfn.CONCAT(A55,"-",B55)</f>
+        <v>CITIES-EXCEL</v>
+      </c>
+      <c r="D55">
+        <v>59</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>199</v>
+      </c>
+      <c r="I55" t="s">
+        <v>199</v>
+      </c>
+      <c r="K55" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" t="str">
+        <f>_xlfn.CONCAT(A56,"-",B56)</f>
+        <v>CITIES-PRINT</v>
+      </c>
+      <c r="D56">
+        <v>60</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>199</v>
+      </c>
+      <c r="I56" t="s">
+        <v>199</v>
+      </c>
+      <c r="K56" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" t="str">
+        <f>_xlfn.CONCAT(A57,"-",B57)</f>
+        <v>CITIES-PDF</v>
+      </c>
+      <c r="D57">
+        <v>61</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="G57" t="s">
+        <v>199</v>
+      </c>
+      <c r="I57" t="s">
+        <v>199</v>
+      </c>
+      <c r="K57" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" t="str">
+        <f>_xlfn.CONCAT(A58,"-",B58)</f>
+        <v>TRAINING-CREATE</v>
+      </c>
+      <c r="D58">
+        <v>62</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>62</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="I58" t="s">
+        <v>199</v>
+      </c>
+      <c r="K58" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C59" t="str">
+        <f>_xlfn.CONCAT(A59,"-",B59)</f>
+        <v>TRAINING-READ</v>
+      </c>
+      <c r="D59">
+        <v>63</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>63</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <v>4</v>
+      </c>
+      <c r="I59">
+        <v>4</v>
+      </c>
+      <c r="J59">
+        <f>D59</f>
+        <v>63</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>195</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" t="str">
+        <f>_xlfn.CONCAT(A60,"-",B60)</f>
+        <v>TRAINING-UPDATE</v>
+      </c>
+      <c r="D60">
+        <v>64</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>64</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="I60" t="s">
+        <v>199</v>
+      </c>
+      <c r="K60" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>195</v>
+      </c>
+      <c r="B61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" t="str">
+        <f>_xlfn.CONCAT(A61,"-",B61)</f>
+        <v>TRAINING-DELETE</v>
+      </c>
+      <c r="D61">
+        <v>65</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>65</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="I61" t="s">
+        <v>199</v>
+      </c>
+      <c r="K61" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" t="str">
+        <f>_xlfn.CONCAT(A62,"-",B62)</f>
+        <v>TRAINING-EXCEL</v>
+      </c>
+      <c r="D62">
+        <v>66</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>66</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="I62" t="s">
+        <v>199</v>
+      </c>
+      <c r="K62" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" t="str">
+        <f>_xlfn.CONCAT(A63,"-",B63)</f>
+        <v>TRAINING-PRINT</v>
+      </c>
+      <c r="D63">
+        <v>67</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>67</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="I63" t="s">
+        <v>199</v>
+      </c>
+      <c r="K63" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C64" t="str">
+        <f>_xlfn.CONCAT(A64,"-",B64)</f>
+        <v>TRAINING-PDF</v>
+      </c>
+      <c r="D64">
+        <v>68</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>68</v>
+      </c>
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="I64" t="s">
+        <v>199</v>
+      </c>
+      <c r="K64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" t="str">
+        <f>_xlfn.CONCAT(A65,"-",B65)</f>
+        <v>TRAININGSTEPS-CREATE</v>
+      </c>
+      <c r="D65">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>69</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="I65" t="s">
+        <v>199</v>
+      </c>
+      <c r="K65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>196</v>
+      </c>
+      <c r="B66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C66" t="str">
+        <f>_xlfn.CONCAT(A66,"-",B66)</f>
+        <v>TRAININGSTEPS-READ</v>
+      </c>
+      <c r="D66">
+        <v>70</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>70</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66">
+        <f>D66</f>
+        <v>70</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" t="str">
+        <f>_xlfn.CONCAT(A67,"-",B67)</f>
+        <v>TRAININGSTEPS-UPDATE</v>
+      </c>
+      <c r="D67">
+        <v>71</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>71</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="I67" t="s">
+        <v>199</v>
+      </c>
+      <c r="K67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" t="str">
+        <f>_xlfn.CONCAT(A68,"-",B68)</f>
+        <v>TRAININGSTEPS-DELETE</v>
+      </c>
+      <c r="D68">
+        <v>72</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>72</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="I68" t="s">
+        <v>199</v>
+      </c>
+      <c r="K68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>196</v>
+      </c>
+      <c r="B69" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" t="str">
+        <f>_xlfn.CONCAT(A69,"-",B69)</f>
+        <v>TRAININGSTEPS-EXCEL</v>
+      </c>
+      <c r="D69">
+        <v>73</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <v>73</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="I69" t="s">
+        <v>199</v>
+      </c>
+      <c r="K69" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>196</v>
+      </c>
+      <c r="B70" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" t="str">
+        <f>_xlfn.CONCAT(A70,"-",B70)</f>
+        <v>TRAININGSTEPS-PRINT</v>
+      </c>
+      <c r="D70">
+        <v>74</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>74</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="I70" t="s">
+        <v>199</v>
+      </c>
+      <c r="K70" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" t="str">
+        <f>_xlfn.CONCAT(A71,"-",B71)</f>
+        <v>TRAININGSTEPS-PDF</v>
+      </c>
+      <c r="D71">
+        <v>75</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <v>75</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="I71" t="s">
+        <v>199</v>
+      </c>
+      <c r="K71" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>197</v>
+      </c>
+      <c r="B72" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" t="str">
+        <f>_xlfn.CONCAT(A72,"-",B72)</f>
+        <v>USERANIMAL-CREATE</v>
+      </c>
+      <c r="D72">
+        <v>76</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="G72" t="s">
+        <v>199</v>
+      </c>
+      <c r="I72" t="s">
+        <v>199</v>
+      </c>
+      <c r="J72">
+        <f>D72</f>
+        <v>76</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>197</v>
+      </c>
+      <c r="B73" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" t="str">
+        <f>_xlfn.CONCAT(A73,"-",B73)</f>
+        <v>USERANIMAL-READ</v>
+      </c>
+      <c r="D73">
+        <v>77</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>77</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>6</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+      <c r="J73">
+        <f>D73</f>
+        <v>77</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" t="str">
+        <f>_xlfn.CONCAT(A74,"-",B74)</f>
+        <v>USERANIMAL-UPDATE</v>
+      </c>
+      <c r="D74">
+        <v>78</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="G74" t="s">
+        <v>199</v>
+      </c>
+      <c r="I74" t="s">
+        <v>199</v>
+      </c>
+      <c r="J74">
+        <f>D74</f>
+        <v>78</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>197</v>
+      </c>
+      <c r="B75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" t="str">
+        <f>_xlfn.CONCAT(A75,"-",B75)</f>
+        <v>USERANIMAL-DELETE</v>
+      </c>
+      <c r="D75">
+        <v>79</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>199</v>
+      </c>
+      <c r="I75" t="s">
+        <v>199</v>
+      </c>
+      <c r="K75" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76" t="s">
+        <v>168</v>
+      </c>
+      <c r="C76" t="str">
+        <f>_xlfn.CONCAT(A76,"-",B76)</f>
+        <v>USERANIMAL-EXCEL</v>
+      </c>
+      <c r="D76">
+        <v>80</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>80</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="I76" t="s">
+        <v>199</v>
+      </c>
+      <c r="K76" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>197</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" t="str">
+        <f>_xlfn.CONCAT(A77,"-",B77)</f>
+        <v>USERANIMAL-PRINT</v>
+      </c>
+      <c r="D77">
+        <v>81</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <v>81</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="I77" t="s">
+        <v>199</v>
+      </c>
+      <c r="K77" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" t="str">
+        <f>_xlfn.CONCAT(A78,"-",B78)</f>
+        <v>USERANIMAL-PDF</v>
+      </c>
+      <c r="D78">
+        <v>82</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>82</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
+      <c r="I78" t="s">
+        <v>199</v>
+      </c>
+      <c r="K78" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" t="str">
+        <f>_xlfn.CONCAT(A79,"-",B79)</f>
+        <v>CAREANNOUNCEMENT-CREATE</v>
+      </c>
+      <c r="D79">
+        <v>83</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="G79" t="s">
+        <v>199</v>
+      </c>
+      <c r="I79" t="s">
+        <v>199</v>
+      </c>
+      <c r="K79" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" t="str">
+        <f>_xlfn.CONCAT(A80,"-",B80)</f>
+        <v>CAREANNOUNCEMENT-READ</v>
+      </c>
+      <c r="D80">
+        <v>84</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="G80" t="s">
+        <v>199</v>
+      </c>
+      <c r="H80">
+        <v>84</v>
+      </c>
+      <c r="I80">
+        <v>4</v>
+      </c>
+      <c r="J80">
+        <f>D80</f>
+        <v>84</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>198</v>
+      </c>
+      <c r="B81" t="s">
+        <v>188</v>
+      </c>
+      <c r="C81" t="str">
+        <f>_xlfn.CONCAT(A81,"-",B81)</f>
+        <v>CAREANNOUNCEMENT-UPDATE</v>
+      </c>
+      <c r="D81">
+        <v>85</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="G81" t="s">
+        <v>199</v>
+      </c>
+      <c r="I81" t="s">
+        <v>199</v>
+      </c>
+      <c r="K81" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>198</v>
+      </c>
+      <c r="B82" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" t="str">
+        <f>_xlfn.CONCAT(A82,"-",B82)</f>
+        <v>CAREANNOUNCEMENT-DELETE</v>
+      </c>
+      <c r="D82">
+        <v>86</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="G82" t="s">
+        <v>199</v>
+      </c>
+      <c r="I82" t="s">
+        <v>199</v>
+      </c>
+      <c r="K82" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>198</v>
+      </c>
+      <c r="B83" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" t="str">
+        <f>_xlfn.CONCAT(A83,"-",B83)</f>
+        <v>CAREANNOUNCEMENT-EXCEL</v>
+      </c>
+      <c r="D83">
+        <v>87</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="G83" t="s">
+        <v>199</v>
+      </c>
+      <c r="I83" t="s">
+        <v>199</v>
+      </c>
+      <c r="K83" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>198</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84" t="str">
+        <f>_xlfn.CONCAT(A84,"-",B84)</f>
+        <v>CAREANNOUNCEMENT-PRINT</v>
+      </c>
+      <c r="D84">
+        <v>88</v>
+      </c>
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="G84" t="s">
+        <v>199</v>
+      </c>
+      <c r="I84" t="s">
+        <v>199</v>
+      </c>
+      <c r="K84" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" t="str">
+        <f>_xlfn.CONCAT(A85,"-",B85)</f>
+        <v>CAREANNOUNCEMENT-PDF</v>
+      </c>
+      <c r="D85">
+        <v>89</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>199</v>
+      </c>
+      <c r="I85" t="s">
+        <v>199</v>
+      </c>
+      <c r="K85" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>200</v>
+      </c>
+      <c r="B86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" t="str">
+        <f>_xlfn.CONCAT(A86,"-",B86)</f>
+        <v>TIMEUNITS-CREATE</v>
+      </c>
+      <c r="D86">
+        <v>90</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="G86" t="s">
+        <v>199</v>
+      </c>
+      <c r="I86" t="s">
+        <v>199</v>
+      </c>
+      <c r="K86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" t="str">
+        <f>_xlfn.CONCAT(A87,"-",B87)</f>
+        <v>TIMEUNITS-READ</v>
+      </c>
+      <c r="D87">
+        <v>91</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="G87" t="s">
+        <v>199</v>
+      </c>
+      <c r="H87">
+        <v>91</v>
+      </c>
+      <c r="I87">
+        <v>4</v>
+      </c>
+      <c r="J87">
+        <f>D87</f>
+        <v>91</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>200</v>
+      </c>
+      <c r="B88" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" t="str">
+        <f>_xlfn.CONCAT(A88,"-",B88)</f>
+        <v>TIMEUNITS-UPDATE</v>
+      </c>
+      <c r="D88">
+        <v>92</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="G88" t="s">
+        <v>199</v>
+      </c>
+      <c r="I88" t="s">
+        <v>199</v>
+      </c>
+      <c r="K88" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" t="str">
+        <f>_xlfn.CONCAT(A89,"-",B89)</f>
+        <v>TIMEUNITS-DELETE</v>
+      </c>
+      <c r="D89">
+        <v>93</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="G89" t="s">
+        <v>199</v>
+      </c>
+      <c r="I89" t="s">
+        <v>199</v>
+      </c>
+      <c r="K89" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>200</v>
+      </c>
+      <c r="B90" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" t="str">
+        <f>_xlfn.CONCAT(A90,"-",B90)</f>
+        <v>TIMEUNITS-EXCEL</v>
+      </c>
+      <c r="D90">
+        <v>94</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="G90" t="s">
+        <v>199</v>
+      </c>
+      <c r="I90" t="s">
+        <v>199</v>
+      </c>
+      <c r="K90" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>200</v>
+      </c>
+      <c r="B91" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" t="str">
+        <f>_xlfn.CONCAT(A91,"-",B91)</f>
+        <v>TIMEUNITS-PRINT</v>
+      </c>
+      <c r="D91">
+        <v>95</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="G91" t="s">
+        <v>199</v>
+      </c>
+      <c r="I91" t="s">
+        <v>199</v>
+      </c>
+      <c r="K91" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>200</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" t="str">
+        <f>_xlfn.CONCAT(A92,"-",B92)</f>
+        <v>TIMEUNITS-PDF</v>
+      </c>
+      <c r="D92">
+        <v>96</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="G92" t="s">
+        <v>199</v>
+      </c>
+      <c r="I92" t="s">
+        <v>199</v>
+      </c>
+      <c r="K92" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K92">
+    <sortCondition ref="D2:D92"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98F56AF-0FBF-4148-86D6-676CB13F090E}">
   <dimension ref="A1:U19"/>
   <sheetViews>
@@ -10069,7 +12848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F251A146-35D4-4760-93E6-A9856726555B}">
   <dimension ref="A1:AM42"/>
   <sheetViews>
@@ -12029,7 +14808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF88E9-A3E8-46CD-AC47-76C4FA16F352}">
   <dimension ref="A1:AA125"/>
   <sheetViews>

</xml_diff>